<commit_message>
write results during run, smallest graph first now
</commit_message>
<xml_diff>
--- a/IE_models/Randlestown_West_Deck_Bridge.xlsx
+++ b/IE_models/Randlestown_West_Deck_Bridge.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Julian/Documents/WorkDocuments/Python/IEmodelV2/IE_models/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Julian/Documents/WorkDocuments/Python/agnetwork/IE_models/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4957CD66-E3BC-2B42-B8D2-FFE4F151F07A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{741D3A9F-0DE5-E343-BF15-198BACDA2A05}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16060" activeTab="1" xr2:uid="{41EF06E5-D224-AC48-85A7-03741ACF90EC}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16060" xr2:uid="{41EF06E5-D224-AC48-85A7-03741ACF90EC}"/>
   </bookViews>
   <sheets>
     <sheet name="Elements" sheetId="1" r:id="rId1"/>
@@ -688,7 +688,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1219,11 +1219,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56EA39B3-DC91-914B-9042-786A21D22A90}">
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="16.33203125" style="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" style="6"/>
@@ -1238,7 +1238,7 @@
     <col min="11" max="16384" width="11" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="17">
       <c r="A1" s="6" t="s">
         <v>2</v>
       </c>
@@ -1270,7 +1270,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" ht="51">
       <c r="A2" s="6" t="s">
         <v>23</v>
       </c>
@@ -1302,7 +1302,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" ht="51">
       <c r="A3" s="6" t="s">
         <v>115</v>
       </c>
@@ -1334,7 +1334,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" ht="51">
       <c r="A4" s="6" t="s">
         <v>24</v>
       </c>
@@ -1366,7 +1366,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="49" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" ht="49" customHeight="1">
       <c r="A5" s="6" t="s">
         <v>203</v>
       </c>
@@ -1398,7 +1398,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" ht="51">
       <c r="A6" s="6" t="s">
         <v>27</v>
       </c>
@@ -1430,7 +1430,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" ht="51">
       <c r="A7" s="6" t="s">
         <v>26</v>
       </c>
@@ -1462,7 +1462,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" ht="51">
       <c r="A8" s="6" t="s">
         <v>26</v>
       </c>
@@ -1492,7 +1492,7 @@
       </c>
       <c r="J8" s="17"/>
     </row>
-    <row r="9" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" ht="51">
       <c r="A9" s="6" t="s">
         <v>26</v>
       </c>
@@ -1522,7 +1522,7 @@
       </c>
       <c r="J9" s="17"/>
     </row>
-    <row r="10" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" ht="51">
       <c r="A10" s="6" t="s">
         <v>26</v>
       </c>
@@ -1552,7 +1552,7 @@
       </c>
       <c r="J10" s="17"/>
     </row>
-    <row r="11" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" ht="51">
       <c r="A11" s="6" t="s">
         <v>25</v>
       </c>
@@ -1584,7 +1584,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="68" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" ht="68">
       <c r="A12" s="6" t="s">
         <v>53</v>
       </c>
@@ -1616,7 +1616,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" ht="51">
       <c r="A13" s="6" t="s">
         <v>28</v>
       </c>
@@ -1648,7 +1648,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" ht="51">
       <c r="A14" s="6" t="s">
         <v>28</v>
       </c>
@@ -1680,7 +1680,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" ht="51">
       <c r="A15" s="6" t="s">
         <v>28</v>
       </c>
@@ -1712,7 +1712,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="16" spans="1:10" s="14" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" s="14" customFormat="1" ht="51">
       <c r="A16" s="14" t="s">
         <v>28</v>
       </c>
@@ -1744,7 +1744,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:10" ht="51">
       <c r="A17" s="6" t="s">
         <v>28</v>
       </c>
@@ -1776,7 +1776,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="85" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:10" ht="85">
       <c r="A18" s="6" t="s">
         <v>54</v>
       </c>
@@ -1808,7 +1808,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:10" ht="51">
       <c r="A19" s="6" t="s">
         <v>29</v>
       </c>
@@ -1840,7 +1840,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:10" ht="51">
       <c r="A20" s="6" t="s">
         <v>29</v>
       </c>
@@ -1872,7 +1872,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:10" ht="51">
       <c r="A21" s="6" t="s">
         <v>29</v>
       </c>
@@ -1904,7 +1904,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="22" spans="1:10" s="15" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:10" s="15" customFormat="1" ht="51">
       <c r="A22" s="15" t="s">
         <v>29</v>
       </c>
@@ -1936,7 +1936,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" ht="51">
       <c r="A23" s="6" t="s">
         <v>29</v>
       </c>
@@ -1968,7 +1968,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="68" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:10" ht="68">
       <c r="A24" s="6" t="s">
         <v>55</v>
       </c>
@@ -2000,7 +2000,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="68" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:10" ht="68">
       <c r="A25" s="6" t="s">
         <v>30</v>
       </c>
@@ -2032,7 +2032,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" ht="51">
       <c r="A26" s="6" t="s">
         <v>62</v>
       </c>
@@ -2064,7 +2064,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" ht="51">
       <c r="A27" s="6" t="s">
         <v>63</v>
       </c>
@@ -2109,17 +2109,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2076CE62-05A5-B445-85CA-61E02B12840C}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3:XFD4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -2130,7 +2130,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3">
       <c r="A2" s="3" t="s">
         <v>11</v>
       </c>
@@ -2154,7 +2154,7 @@
       <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="2" width="11" style="2"/>
     <col min="3" max="3" width="11.33203125" style="2" customWidth="1"/>
@@ -2167,7 +2167,7 @@
     <col min="26" max="26" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:26" s="1" customFormat="1">
       <c r="A1" s="7" t="s">
         <v>5</v>
       </c>
@@ -2212,7 +2212,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:26">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -2252,7 +2252,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:26">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -2292,7 +2292,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="4" spans="1:26" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" ht="17" thickBot="1">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -2334,7 +2334,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:26" ht="15.75" customHeight="1">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -2378,7 +2378,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:26">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -2420,7 +2420,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:26">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -2462,7 +2462,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:26">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -2504,7 +2504,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" ht="17" thickBot="1">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -2546,7 +2546,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:26">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -2584,7 +2584,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" ht="17" thickBot="1">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -2622,7 +2622,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="12" spans="1:26" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" ht="17" thickBot="1">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -2653,7 +2653,7 @@
         <v>57.479000000000006</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:26">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -2677,7 +2677,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:26">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -2701,7 +2701,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:26">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -2725,7 +2725,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:26">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -2749,7 +2749,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -2773,7 +2773,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -2797,7 +2797,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -2821,7 +2821,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -2845,7 +2845,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:9">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -2868,7 +2868,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -2891,7 +2891,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -2914,7 +2914,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -2937,7 +2937,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -2960,7 +2960,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -2984,7 +2984,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -3008,7 +3008,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9">
       <c r="A28" s="2">
         <v>27</v>
       </c>
@@ -3032,7 +3032,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -3056,7 +3056,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:9">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -3080,7 +3080,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:9">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -3104,7 +3104,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9">
       <c r="A32" s="2">
         <v>31</v>
       </c>
@@ -3128,7 +3128,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -3152,7 +3152,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9">
       <c r="A34" s="2">
         <v>33</v>
       </c>
@@ -3176,7 +3176,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9">
       <c r="A35" s="2">
         <v>34</v>
       </c>
@@ -3200,7 +3200,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9">
       <c r="A36" s="2">
         <v>35</v>
       </c>
@@ -3224,7 +3224,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9">
       <c r="A37" s="2">
         <v>36</v>
       </c>
@@ -3248,7 +3248,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9">
       <c r="A38" s="2">
         <v>37</v>
       </c>
@@ -3272,7 +3272,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:9">
       <c r="A39" s="2">
         <v>38</v>
       </c>
@@ -3296,7 +3296,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:9">
       <c r="A40" s="2">
         <v>39</v>
       </c>
@@ -3320,7 +3320,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:9">
       <c r="A41" s="2">
         <v>40</v>
       </c>
@@ -3344,7 +3344,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:9">
       <c r="A42" s="2">
         <v>41</v>
       </c>
@@ -3368,7 +3368,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:9">
       <c r="A43" s="2">
         <v>42</v>
       </c>
@@ -3392,7 +3392,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:9">
       <c r="A44" s="2">
         <v>43</v>
       </c>
@@ -3416,7 +3416,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:9">
       <c r="A45" s="2">
         <v>44</v>
       </c>
@@ -3440,7 +3440,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:9">
       <c r="A46" s="2">
         <v>45</v>
       </c>
@@ -3464,7 +3464,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:9">
       <c r="A47" s="2">
         <v>46</v>
       </c>
@@ -3488,7 +3488,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:9">
       <c r="A48" s="2">
         <v>47</v>
       </c>
@@ -3511,7 +3511,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:9">
       <c r="A49" s="2">
         <v>48</v>
       </c>
@@ -3535,7 +3535,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:9">
       <c r="A50" s="2">
         <v>49</v>
       </c>
@@ -3559,7 +3559,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:9">
       <c r="A51" s="2">
         <v>50</v>
       </c>
@@ -3582,7 +3582,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:9">
       <c r="A52" s="2">
         <v>51</v>
       </c>
@@ -3605,7 +3605,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:9">
       <c r="A53" s="2">
         <v>52</v>
       </c>
@@ -3629,7 +3629,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:9">
       <c r="A54" s="2">
         <v>53</v>
       </c>

</xml_diff>

<commit_message>
Not sure what's changed there
</commit_message>
<xml_diff>
--- a/IE_models/Randlestown_West_Deck_Bridge.xlsx
+++ b/IE_models/Randlestown_West_Deck_Bridge.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Julian/Documents/WorkDocuments/Python/agnetwork/IE_models/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{741D3A9F-0DE5-E343-BF15-198BACDA2A05}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6C75429-392A-C840-BEB0-6BD2DDF5A53B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16060" xr2:uid="{41EF06E5-D224-AC48-85A7-03741ACF90EC}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="14780" windowHeight="9600" xr2:uid="{41EF06E5-D224-AC48-85A7-03741ACF90EC}"/>
   </bookViews>
   <sheets>
     <sheet name="Elements" sheetId="1" r:id="rId1"/>
@@ -1219,7 +1219,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56EA39B3-DC91-914B-9042-786A21D22A90}">
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>

</xml_diff>